<commit_message>
12th - In One excel for Zacks
</commit_message>
<xml_diff>
--- a/Reports/MarketBeatRank/TanzyGrowth/TNDM.xlsx
+++ b/Reports/MarketBeatRank/TanzyGrowth/TNDM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10523"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/setup/Desktop/Personal/Finance_Learn_Reports/MarketBeatRank/TanzyGrowth/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/i852841/_Codes/_Personal/StockRankingCrawler/Reports/MarketBeatRank/TanzyGrowth/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{30F13774-CA01-2F4D-B875-D8A27DB38B4A}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33"/>
+  <xr:revisionPtr documentId="13_ncr:1_{F1E49FE2-F3CB-FC49-9767-10B9689BE8CD}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36"/>
   <bookViews>
     <workbookView windowHeight="19700" windowWidth="33600" xWindow="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="460"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1369" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37304" uniqueCount="81">
   <si>
     <t>Jun_10</t>
   </si>
@@ -115,31 +115,154 @@
     <t>2/27/2018,Initiated Coverage,Outperform,$5.50</t>
   </si>
   <si>
+    <t>Jun_26</t>
+  </si>
+  <si>
+    <t>6/22/2018,Upgrades,Overweight,$25.00</t>
+  </si>
+  <si>
+    <t>Benchmark</t>
+  </si>
+  <si>
+    <t>Evercore ISI</t>
+  </si>
+  <si>
+    <t>Aug_14</t>
+  </si>
+  <si>
+    <t>8/14/2018,Upgrades,Sell -&gt; Hold,</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>Jun_13</t>
-  </si>
-  <si>
-    <t>Jun_15</t>
-  </si>
-  <si>
-    <t>Jun_17</t>
-  </si>
-  <si>
-    <t>Jun_26</t>
-  </si>
-  <si>
-    <t>6/22/2018,Upgrades,Overweight,$25.00</t>
-  </si>
-  <si>
-    <t>Benchmark</t>
-  </si>
-  <si>
-    <t>Evercore ISI</t>
-  </si>
-  <si>
-    <t>Jun_27</t>
+    <t>Aug_21</t>
+  </si>
+  <si>
+    <t>Aug_26</t>
+  </si>
+  <si>
+    <t>8/22/2018,Initiates,Hold,$25.00 -&gt; $34.00</t>
+  </si>
+  <si>
+    <t>8/24/2018,Upgrades,Underperform -&gt; Neutral,$45.00</t>
+  </si>
+  <si>
+    <t>8/23/2018,Upgrades,Buy -&gt; Strong-Buy,</t>
+  </si>
+  <si>
+    <t>Sep_02</t>
+  </si>
+  <si>
+    <t>Sep_11</t>
+  </si>
+  <si>
+    <t>Sep_24</t>
+  </si>
+  <si>
+    <t>Oct_01</t>
+  </si>
+  <si>
+    <t>9/26/2018,Reiterates,Above Average -&gt; Overweight,$32.00 -&gt; $56.00</t>
+  </si>
+  <si>
+    <t>Oct_06</t>
+  </si>
+  <si>
+    <t>10/6/2018,Downgrades,Buy -&gt; Hold,</t>
+  </si>
+  <si>
+    <t>Oct_22</t>
+  </si>
+  <si>
+    <t>Nov_04</t>
+  </si>
+  <si>
+    <t>Nov_11</t>
+  </si>
+  <si>
+    <t>11/7/2018,Downgrades,Strong-Buy -&gt; Buy,</t>
+  </si>
+  <si>
+    <t>Nov_19</t>
+  </si>
+  <si>
+    <t>11/15/2018,Downgrades,Buy -&gt; Hold,</t>
+  </si>
+  <si>
+    <t>Nov_24</t>
+  </si>
+  <si>
+    <t>Dec_02</t>
+  </si>
+  <si>
+    <t>Dec_09</t>
+  </si>
+  <si>
+    <t>Dec_16</t>
+  </si>
+  <si>
+    <t>Dec_30</t>
+  </si>
+  <si>
+    <t>12/28/2018,Upgrades,Hold -&gt; Buy,</t>
+  </si>
+  <si>
+    <t>Jan_07</t>
+  </si>
+  <si>
+    <t>Jan_13</t>
+  </si>
+  <si>
+    <t>1/12/2019,Upgrades,Buy -&gt; Strong-Buy,</t>
+  </si>
+  <si>
+    <t>Jan_21</t>
+  </si>
+  <si>
+    <t>Jan_27</t>
+  </si>
+  <si>
+    <t>Jan_31</t>
+  </si>
+  <si>
+    <t>Feb_03</t>
+  </si>
+  <si>
+    <t>Feb_07</t>
+  </si>
+  <si>
+    <t>Feb_10</t>
+  </si>
+  <si>
+    <t>Feb_13</t>
+  </si>
+  <si>
+    <t>Feb_17</t>
+  </si>
+  <si>
+    <t>Feb_24</t>
+  </si>
+  <si>
+    <t>Feb_28</t>
+  </si>
+  <si>
+    <t>2/27/2019,Upgrades,Overweight,$67.00</t>
+  </si>
+  <si>
+    <t>2/28/2019,Downgrades,Strong-Buy -&gt; Buy,</t>
+  </si>
+  <si>
+    <t>Mar_03</t>
+  </si>
+  <si>
+    <t>Mar_06</t>
+  </si>
+  <si>
+    <t>3/5/2019,Reiterates,Neutral,$59.00</t>
+  </si>
+  <si>
+    <t>Mar_10</t>
   </si>
 </sst>
 </file>
@@ -156,12 +279,72 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="22">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="45"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="45"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="45"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="45"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="45"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="45"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="45"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="45"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="none">
@@ -183,6 +366,26 @@
         <fgColor indexed="42"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="45"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="45"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -196,17 +399,29 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+  <cellXfs count="927">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
@@ -235,6 +450,836 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFill="true" borderId="0" fillId="5" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="5" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="7" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="11" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="13" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="15" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="17" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="19" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="21" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
@@ -596,46 +1641,164 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="21.1640625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="39.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="39.0" collapsed="true"/>
     <col min="3" max="3" customWidth="true" width="39.0" collapsed="true"/>
     <col min="4" max="4" customWidth="true" width="39.0" collapsed="true"/>
     <col min="5" max="5" customWidth="true" width="39.0" collapsed="true"/>
     <col min="6" max="6" customWidth="true" width="39.0" collapsed="true"/>
     <col min="7" max="7" customWidth="true" width="39.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="39.0" collapsed="false"/>
+    <col min="8" max="8" customWidth="true" width="39.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="39.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="39.0" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="39.0" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="39.0" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="39.0" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="39.0" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="39.0" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="39.0" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="39.0" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="39.0" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" width="39.0" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" width="39.0" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" width="39.0" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" width="39.0" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" width="39.0" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" width="39.0" collapsed="true"/>
+    <col min="25" max="25" customWidth="true" width="39.0" collapsed="true"/>
+    <col min="26" max="26" customWidth="true" width="39.0" collapsed="true"/>
+    <col min="27" max="27" customWidth="true" width="39.0" collapsed="true"/>
+    <col min="28" max="28" customWidth="true" width="39.0" collapsed="true"/>
+    <col min="29" max="29" customWidth="true" width="39.0" collapsed="true"/>
+    <col min="30" max="30" customWidth="true" width="39.0" collapsed="true"/>
+    <col min="31" max="31" customWidth="true" width="39.0" collapsed="true"/>
+    <col min="32" max="32" customWidth="true" width="39.0" collapsed="true"/>
+    <col min="33" max="33" customWidth="true" width="39.0" collapsed="true"/>
+    <col min="34" max="34" customWidth="true" width="39.0" collapsed="true"/>
+    <col min="35" max="35" customWidth="true" width="39.0" collapsed="true"/>
+    <col min="36" max="36" customWidth="true" width="39.0" collapsed="true"/>
+    <col min="37" max="37" customWidth="true" width="39.0" collapsed="false"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="P1" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q1" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="R1" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="S1" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="T1" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="U1" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="V1" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="W1" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="X1" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y1" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z1" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA1" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB1" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC1" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="AD1" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="AE1" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="AF1" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="AG1" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="AH1" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="AI1" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="H1" s="0" t="s">
+      <c r="AJ1" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="AK1" s="0" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -660,8 +1823,95 @@
       <c r="H2" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="I2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="M2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="N2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="O2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="P2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="R2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="S2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="T2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="U2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="V2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="W2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="X2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AG2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AK2" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -686,8 +1936,95 @@
       <c r="H3" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="I3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="L3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="M3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="N3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="O3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="P3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="R3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="S3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="T3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="U3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="V3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="W3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="X3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AG3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AK3" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -712,8 +2049,95 @@
       <c r="H4" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="I4" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="L4" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="M4" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="N4" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="O4" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="P4" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q4" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="R4" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="S4" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="T4" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="U4" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="V4" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="W4" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="X4" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y4" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z4" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA4" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB4" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC4" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD4" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE4" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF4" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AG4" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH4" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI4" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ4" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AK4" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -738,8 +2162,95 @@
       <c r="H5" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="I5" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="K5" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="L5" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="M5" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="N5" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="O5" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="P5" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q5" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="R5" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="S5" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="T5" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="U5" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="V5" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="W5" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="X5" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y5" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z5" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA5" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB5" s="174" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC5" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD5" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE5" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF5" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AG5" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH5" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AJ5" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AK5" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -764,8 +2275,95 @@
       <c r="H6" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="I6" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="K6" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="L6" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="M6" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="N6" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="O6" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="P6" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q6" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="R6" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="S6" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="T6" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="U6" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="V6" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="W6" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="X6" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y6" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z6" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA6" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB6" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC6" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD6" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE6" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF6" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AG6" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH6" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI6" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ6" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AK6" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -790,8 +2388,95 @@
       <c r="H7" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="I7" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="J7" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="K7" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="L7" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="M7" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="N7" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="O7" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="P7" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q7" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="R7" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="S7" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="T7" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="U7" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="V7" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="W7" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="X7" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y7" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z7" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA7" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB7" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC7" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD7" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE7" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF7" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AG7" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH7" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI7" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ7" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AK7" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -816,8 +2501,95 @@
       <c r="H8" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="I8" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="J8" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="K8" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="L8" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="M8" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="N8" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="O8" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="P8" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q8" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="R8" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="S8" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="T8" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="U8" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="V8" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="W8" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="X8" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y8" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z8" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA8" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB8" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC8" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD8" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE8" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF8" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AG8" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH8" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI8" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ8" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AK8" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -842,22 +2614,109 @@
       <c r="H9" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="I9" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="J9" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="K9" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="L9" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="M9" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="N9" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="O9" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="P9" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q9" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="R9" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="S9" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="T9" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="U9" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="V9" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="W9" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="X9" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y9" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z9" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA9" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB9" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC9" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD9" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE9" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF9" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AG9" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH9" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI9" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ9" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AK9" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="B10" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="37" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>2</v>
+      <c r="C10" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="823" t="s">
+        <v>75</v>
       </c>
       <c r="F10" s="0" t="s">
         <v>2</v>
@@ -866,10 +2725,97 @@
         <v>2</v>
       </c>
       <c r="H10" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="I10" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="J10" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="K10" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="L10" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="M10" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="N10" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="O10" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="P10" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q10" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="R10" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="S10" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="T10" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="U10" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="V10" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="W10" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="X10" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y10" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z10" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA10" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB10" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC10" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="AD10" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE10" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF10" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AG10" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH10" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI10" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AK10" s="0" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -882,8 +2828,8 @@
       <c r="D11" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="E11" s="0" t="s">
-        <v>2</v>
+      <c r="E11" s="824" t="s">
+        <v>76</v>
       </c>
       <c r="F11" s="0" t="s">
         <v>2</v>
@@ -894,8 +2840,95 @@
       <c r="H11" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="I11" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="J11" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="K11" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="L11" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="M11" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="N11" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="O11" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="P11" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q11" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="R11" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="S11" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="T11" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="U11" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="V11" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="W11" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="X11" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y11" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z11" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA11" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB11" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC11" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD11" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE11" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF11" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AG11" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH11" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI11" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ11" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AK11" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -920,8 +2953,95 @@
       <c r="H12" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="I12" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="J12" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="K12" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="L12" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="M12" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="N12" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="O12" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="P12" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q12" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="R12" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="S12" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="T12" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="U12" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="V12" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="W12" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="X12" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y12" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z12" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA12" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB12" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC12" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD12" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE12" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF12" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AG12" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH12" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI12" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ12" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AK12" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -946,8 +3066,95 @@
       <c r="H13" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="I13" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="J13" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="K13" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="L13" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="M13" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="N13" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="O13" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="P13" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q13" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="R13" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="S13" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="T13" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="U13" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="V13" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="W13" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="X13" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y13" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z13" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA13" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB13" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC13" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD13" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE13" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF13" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AG13" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH13" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI13" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ13" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AK13" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -970,10 +3177,97 @@
         <v>2</v>
       </c>
       <c r="H14" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="I14" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="J14" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="K14" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="L14" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="M14" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="N14" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="O14" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="P14" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q14" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="R14" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="S14" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="T14" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="U14" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="V14" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="W14" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="X14" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y14" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z14" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA14" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB14" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC14" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD14" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE14" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF14" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AG14" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="AH14" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI14" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ14" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AK14" s="0" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -998,8 +3292,95 @@
       <c r="H15" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="I15" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="J15" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="K15" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="L15" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="M15" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="N15" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="O15" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="P15" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q15" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="R15" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="S15" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="T15" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="U15" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="V15" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="W15" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="X15" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y15" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z15" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA15" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB15" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC15" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD15" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE15" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF15" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AG15" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH15" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI15" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ15" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AK15" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -1024,8 +3405,95 @@
       <c r="H16" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="I16" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="J16" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="K16" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="L16" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="M16" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="N16" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="O16" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="P16" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q16" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="R16" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="S16" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="T16" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="U16" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="V16" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="W16" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="X16" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y16" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z16" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA16" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB16" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC16" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD16" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE16" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF16" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AG16" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH16" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI16" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ16" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AK16" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -1050,8 +3518,95 @@
       <c r="H17" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="I17" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="J17" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="K17" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="L17" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="M17" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="N17" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="O17" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="P17" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q17" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="R17" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="S17" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="T17" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="U17" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="V17" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="W17" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="X17" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y17" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z17" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA17" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB17" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC17" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD17" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE17" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF17" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AG17" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH17" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI17" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ17" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AK17" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -1076,8 +3631,95 @@
       <c r="H18" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="I18" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="J18" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="K18" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="L18" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="M18" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="N18" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="O18" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="P18" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q18" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="R18" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="S18" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="T18" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="U18" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="V18" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="W18" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="X18" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y18" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z18" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA18" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB18" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC18" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD18" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE18" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF18" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AG18" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH18" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI18" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ18" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AK18" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -1100,10 +3742,97 @@
         <v>2</v>
       </c>
       <c r="H19" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="I19" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="J19" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="K19" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="L19" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="M19" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="N19" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="O19" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="P19" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q19" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="R19" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="S19" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="T19" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="U19" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="V19" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="W19" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="X19" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y19" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z19" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA19" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB19" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC19" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD19" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE19" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF19" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AG19" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH19" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI19" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ19" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AK19" s="0" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -1111,7 +3840,7 @@
         <v>2</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>2</v>
+        <v>79</v>
       </c>
       <c r="D20" s="0" t="s">
         <v>2</v>
@@ -1128,8 +3857,95 @@
       <c r="H20" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="I20" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="J20" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="K20" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="L20" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="M20" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="N20" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="O20" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="P20" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q20" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="R20" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="S20" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="T20" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="U20" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="V20" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="W20" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="X20" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y20" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z20" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA20" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB20" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC20" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD20" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE20" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF20" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AG20" s="49" t="s">
+        <v>41</v>
+      </c>
+      <c r="AH20" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI20" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ20" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AK20" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -1154,8 +3970,95 @@
       <c r="H21" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="I21" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="J21" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="K21" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="L21" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="M21" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="N21" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="O21" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="P21" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q21" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="R21" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="S21" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="T21" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="U21" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="V21" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="W21" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="X21" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y21" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z21" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA21" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB21" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC21" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD21" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE21" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF21" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AG21" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH21" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI21" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ21" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AK21" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -1180,8 +4083,95 @@
       <c r="H22" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="I22" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="J22" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="K22" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="L22" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="M22" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="N22" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="O22" s="555" t="s">
+        <v>64</v>
+      </c>
+      <c r="P22" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q22" s="499" t="s">
+        <v>61</v>
+      </c>
+      <c r="R22" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="S22" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="T22" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="U22" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="V22" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="W22" s="331" t="s">
+        <v>55</v>
+      </c>
+      <c r="X22" s="303" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y22" s="275" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z22" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA22" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB22" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC22" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD22" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE22" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF22" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AG22" s="51" t="s">
+        <v>42</v>
+      </c>
+      <c r="AH22" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI22" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ22" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AK22" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -1206,8 +4196,95 @@
       <c r="H23" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="I23" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="J23" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="K23" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="L23" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="M23" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="N23" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="O23" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="P23" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q23" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="R23" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="S23" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="T23" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="U23" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="V23" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="W23" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="X23" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y23" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z23" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA23" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB23" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC23" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD23" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE23" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF23" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AG23" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH23" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI23" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ23" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AK23" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -1232,8 +4309,95 @@
       <c r="H24" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="I24" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="J24" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="K24" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="L24" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="M24" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="N24" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="O24" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="P24" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q24" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="R24" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="S24" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="T24" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="U24" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="V24" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="W24" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="X24" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y24" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z24" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA24" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB24" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC24" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD24" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE24" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF24" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AG24" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH24" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI24" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ24" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AK24" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -1258,8 +4422,95 @@
       <c r="H25" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="I25" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="J25" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="K25" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="L25" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="M25" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="N25" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="O25" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="P25" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q25" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="R25" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="S25" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="T25" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="U25" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="V25" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="W25" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="X25" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y25" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z25" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA25" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB25" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC25" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD25" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE25" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF25" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AG25" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH25" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI25" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ25" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AK25" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -1284,8 +4535,95 @@
       <c r="H26" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="I26" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="J26" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="K26" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="L26" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="M26" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="N26" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="O26" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="P26" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q26" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="R26" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="S26" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="T26" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="U26" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="V26" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="W26" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="X26" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y26" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z26" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA26" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB26" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC26" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD26" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE26" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF26" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AG26" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH26" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI26" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ26" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AK26" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>28</v>
       </c>
@@ -1310,10 +4648,97 @@
       <c r="H27" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="I27" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="J27" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="K27" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="L27" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="M27" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="N27" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="O27" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="P27" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q27" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="R27" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="S27" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="T27" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="U27" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="V27" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="W27" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="X27" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y27" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z27" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA27" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB27" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC27" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD27" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE27" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF27" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AG27" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH27" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI27" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ27" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AK27" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B28" t="s">
         <v>2</v>
@@ -1324,10 +4749,106 @@
       <c r="D28" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="E28" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="F28" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="G28" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="H28" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="I28" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="J28" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="K28" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="L28" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="M28" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="N28" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="O28" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="P28" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q28" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="R28" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="S28" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="T28" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="U28" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="V28" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="W28" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="X28" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y28" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z28" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA28" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB28" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC28" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD28" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE28" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF28" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AG28" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH28" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI28" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ28" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B29" t="s">
         <v>2</v>
@@ -1336,6 +4857,102 @@
         <v>2</v>
       </c>
       <c r="D29" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E29" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="F29" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="G29" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="H29" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="I29" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="J29" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="K29" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="L29" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="M29" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="N29" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="O29" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="P29" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q29" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="R29" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="S29" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="T29" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="U29" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="V29" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="W29" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="X29" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y29" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z29" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA29" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB29" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC29" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD29" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE29" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF29" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AG29" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH29" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI29" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ29" s="0" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>